<commit_message>
nytt excel för scape script
</commit_message>
<xml_diff>
--- a/data/scape_bought_by_country.xlsx
+++ b/data/scape_bought_by_country.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:E8"/>
@@ -1514,6 +1514,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>500</v>
+      </c>
+      <c r="C57" t="n">
+        <v>500</v>
+      </c>
+      <c r="D57" t="n">
+        <v>50</v>
+      </c>
+      <c r="E57" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
nytt scape script med fil uppdaterad
</commit_message>
<xml_diff>
--- a/data/scape_bought_by_country.xlsx
+++ b/data/scape_bought_by_country.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:E8"/>
@@ -1590,6 +1590,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-11-29</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>500</v>
+      </c>
+      <c r="C61" t="n">
+        <v>500</v>
+      </c>
+      <c r="D61" t="n">
+        <v>50</v>
+      </c>
+      <c r="E61" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>